<commit_message>
analysing plant height / biomass distribution to inform plot nesting
</commit_message>
<xml_diff>
--- a/Data/GEF Field Trial/GEF_Woody canopy_2017.10.16_Mdoda.xlsx
+++ b/Data/GEF Field Trial/GEF_Woody canopy_2017.10.16_Mdoda.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="INT-01" sheetId="10" r:id="rId1"/>
@@ -5723,8 +5723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L127"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6355,6 +6355,15 @@
       <c r="B43" t="s">
         <v>49</v>
       </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
@@ -7553,8 +7562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>